<commit_message>
Add table with bad roll column to test_workbook.xlsx and a code to run stanza to add this new table to the ones checked to test new internal function _check_roll_column().
</commit_message>
<xml_diff>
--- a/data/test_workbook.xlsx
+++ b/data/test_workbook.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Users\valen\Documents\Valen\python\python-repository\npc-generator\my_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Users\valen\Documents\Valen\python\python-repository\npc-generator\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4EAAF70-D2B5-49FF-B432-B1A8EDAEE840}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB9DAFDB-8D14-4B58-905E-6997ED8A821B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3375" yWindow="3375" windowWidth="21600" windowHeight="11295" firstSheet="2" activeTab="2" xr2:uid="{C7386903-D618-4170-9A19-EF0E6AE053B0}"/>
+    <workbookView xWindow="1950" yWindow="1950" windowWidth="10410" windowHeight="11295" firstSheet="6" activeTab="6" xr2:uid="{C7386903-D618-4170-9A19-EF0E6AE053B0}"/>
   </bookViews>
   <sheets>
     <sheet name="Treasure For CR 0 Magic" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="Treasure For CRs 3-4 Coin" sheetId="4" r:id="rId4"/>
     <sheet name="Treasure For CRs 3-4 Magic" sheetId="5" r:id="rId5"/>
     <sheet name="Treasure For CR 0 Coin" sheetId="6" r:id="rId6"/>
+    <sheet name="Treasure For CR 5 Coin" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="25">
   <si>
     <t>D20</t>
   </si>
@@ -113,6 +114,9 @@
   </si>
   <si>
     <t>8-19</t>
+  </si>
+  <si>
+    <t>3D20</t>
   </si>
 </sst>
 </file>
@@ -192,9 +196,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -232,7 +236,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -338,7 +342,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -480,7 +484,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -616,7 +620,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{070E22D2-74FD-4338-A6B2-96C3597B94E0}">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -870,4 +874,73 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B2F8B5F-DCFD-42A1-9B24-F307DFAB23D8}">
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>